<commit_message>
Committed after changing files of OCM audio video play back report
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/AgentHistoricalReportData.xlsx
+++ b/ocms/src/test/resources/TestData/AgentHistoricalReportData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA07302-17DA-4572-A11E-ADEC75E6148E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF043346-03E6-4912-BFE9-747C9ED13F9A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="33">
   <si>
     <t>Report Channel</t>
   </si>
@@ -120,6 +120,44 @@
   </si>
   <si>
     <t>11-05-2020 00:00:00</t>
+  </si>
+  <si>
+    <t>SELECT M.AgentID as [Agent ID],A.AgentName as[Agent Name],A.TeamName as [Team Name],A.SupervisorName as[Supervisor Name],sum(ACDCalls) AS [Total Interaction],[dbo].[SECONDSTOhhmmss](SUM([TotalInteractionTime])) as [Total Interaction Time],
+[dbo].[SECONDSTOhhmmss](SUM([TotalInteractionTime])/nullif(SUM(ACDCalls),0))AS [Avg Interaction Time],SUM([TotalChat]) as [Total Chat],
+[dbo].[SECONDSTOhhmmss](SUM([TotalChatTime])) as[Total Chat Time],[dbo].[SECONDSTOhhmmss](SUM([TotalChatTime])/nullif(sum([TotalChat]),0))AS [Avg Chat Time],SUM([TotalAudioIP]) as [Total Audio IP],[dbo].[SECONDSTOhhmmss](sum([TotalAudioIPTime])) [Total AudioIP Time],
+[dbo].[SECONDSTOhhmmss](SUM([TotalAudioIPTime])/nullif(SUM([TotalAudioIP]),0))AS [Avg AudioIP Time],
+[dbo].[SECONDSTOhhmmss](SUM(TotalInteractionTime)/nullif(SUM(ACDCalls),0))AS [Avg Talk Time],[dbo].[SECONDSTOhhmmss](SUM(TotalAfterCallTime)) as [Total After Call Time],[dbo].[SECONDSTOhhmmss](SUM(TotalAvailTime)) as [Total Avail Time],[dbo].[SECONDSTOhhmmss](SUM(TotalAuxTime)) as [Total AUX Time],SUM(ExtensionCalls) AS [Extension Interaction],[dbo].[SECONDSTOhhmmss](sum([TotalExtensionTime])) as [Total Extension Time],
+[dbo].[SECONDSTOhhmmss](sum(TotalExtensionTime)/nullif(sum(ExtensionCalls),0))AS [Avg Extension Time],[dbo].[SECONDSTOhhmmss](SUM(TotalStaffedTime)) as [Total Time Staffed],[dbo].[SECONDSTOhhmmss](SUM(TotalHoldTime)) as [Total Hold Time] 
+FROM [OCM_AgentHistoricalReport] M WITH(NOLOCK)
+INNER JOIN fn_AgentHierarchy('na','1','1') A ON  A.[AgentId]=M.[AgentID]
+WHERE [ReportDateTime]&gt;='ReportBeforeDate' and [ReportDateTime]&lt;='ReportAfterDate'
+GROUP BY M.[AgentID], A.[AgentName],A.[TeamName],A.[SupervisorName]
+Order by [Agent Name];</t>
+  </si>
+  <si>
+    <t>SELECT Dateint AS [Date],AgentID as [Agent ID],ISNULL(A.FirstName,'')+' '+ ISNULL(A.LastName,'') AS [Agent Name],ISNULL(C.TeamName,' ') AS TeamName,
+ISNULL(B.FirstName,'NA')+' '+ ISNULL(B.LastName,'') AS SupervisorName,SUM(ACDCalls) AS TotalInteraction,
+[dbo].[SECONDSTOhhmmss](SUM([TotalInteractionTime])) [Total Interaction Time],
+[dbo].[SECONDSTOhhmmss](SUM([TotalInteractionTime])/nullif(SUM(ACDCalls),0))AS [Avg Interaction Time],
+SUM([TotalChat]) as [Total Chat],[dbo].[SECONDSTOhhmmss](SUM([TotalChatTime])) as [Total Chat Time],
+[dbo].[SECONDSTOhhmmss](SUM([TotalChatTime])/nullif(sum([TotalChat]),0))AS [Avg Chat Time],
+SUM([TotalAudioIP]) [Total Audio IP],[dbo].[SECONDSTOhhmmss](sum([TotalAudioIPTime])) [Total AudioIP Time],
+[dbo].[SECONDSTOhhmmss](SUM([TotalAudioIPTime])/nullif(SUM([TotalAudioIP]),0))AS [Avg AudioIP Time],
+[dbo].[SECONDSTOhhmmss](SUM(TotalInteractionTime)/nullif(SUM(ACDCalls),0))AS [Avg Talk Time],
+[dbo].[SECONDSTOhhmmss](SUM(TotalAfterCallTime)) as [Total After Call Time],
+[dbo].[SECONDSTOhhmmss](SUM(TotalAvailTime)) as [Total Avail Time],
+[dbo].[SECONDSTOhhmmss](SUM(TotalAuxTime)) as [Total Aux Time],
+SUM(ExtensionCalls) AS [Extension Interaction],
+[dbo].[SECONDSTOhhmmss](sum([TotalExtensionTime])) [Total Extension Time],
+[dbo].[SECONDSTOhhmmss](sum(TotalExtensionTime)/nullif(sum(ExtensionCalls),0))AS [Avg Extension Time],
+[dbo].[SECONDSTOhhmmss](SUM(TotalStaffedTime)) as [Total Time Staffed],
+[dbo].[SECONDSTOhhmmss](SUM(TotalHoldTime)) as [Total Hold Time]  
+FROM [OCM_AgentHistoricalReport] M WITH(NOLOCK)
+LEFT JOIN [AGT_Agent] A WITH(NOLOCK)  ON A.AvayaLoginID = M.[AgentID] 
+LEFT JOIN [AGT_Agent] B WITH(NOLOCK)  ON A.[PrimarySupervisorID]=B.ID LEFT JOIN [AGT_Teams] C WITH(NOLOCK) ON C.TeamID = A.TeamID
+LEFT JOIN[dbo].[AGT_Teams] P WITH(NOLOCK) ON C.ParentID = P.TeamID 
+WHERE [ReportDateTime]&gt;='ReportBeforeDate' AND [ReportDateTime]&lt;='ReportAfterDate' AND [AgentID] LIKE 'AgentIdCapturedFromUI'  
+GROUP BY  [Dateint], [AgentID],B.[FirstName],B.[LastName],C.TeamName,A.FirstName,A.LastName ORDER BY [Dateint] ASC;</t>
   </si>
 </sst>
 </file>
@@ -155,10 +193,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F093AD83-E38D-48DA-BA71-06BDB2F31AEB}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -656,8 +700,8 @@
     <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="82.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.54296875" customWidth="1"/>
     <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -687,7 +731,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -702,6 +746,12 @@
       </c>
       <c r="E2" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit Reports Fixed 03/09/2021
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/AgentHistoricalReportData.xlsx
+++ b/ocms/src/test/resources/TestData/AgentHistoricalReportData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2200C5B9-9EE7-4303-BE44-C731C84035BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1816559-C8EF-445F-9BF6-A9F48DD0B611}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Show" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="56">
   <si>
     <t>Report Channel</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>Villers</t>
-  </si>
-  <si>
-    <t>Am</t>
   </si>
   <si>
     <t>Abrahma Villers</t>
@@ -240,6 +237,18 @@
   </si>
   <si>
     <t>22-05-2020 00:00:00</t>
+  </si>
+  <si>
+    <t>DeleteReason</t>
+  </si>
+  <si>
+    <t>Deleted</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Med</t>
   </si>
 </sst>
 </file>
@@ -570,21 +579,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,8 +607,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -610,6 +623,9 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -620,24 +636,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" customWidth="1"/>
-    <col min="7" max="7" width="22.453125" customWidth="1"/>
-    <col min="8" max="8" width="23.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,8 +679,11 @@
       <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+      <c r="I1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -674,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
@@ -686,10 +706,13 @@
         <v>16</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -700,7 +723,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>23</v>
@@ -715,7 +738,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -726,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>23</v>
@@ -741,7 +764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -752,7 +775,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>23</v>
@@ -764,10 +787,10 @@
         <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -778,13 +801,13 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
@@ -800,21 +823,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.21875" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -827,32 +850,34 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>42</v>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C6" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -867,15 +892,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -892,7 +917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -903,7 +928,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
@@ -922,15 +947,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -944,7 +969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -971,15 +996,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -996,7 +1021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1007,7 +1032,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
@@ -1023,22 +1048,22 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" customWidth="1"/>
-    <col min="7" max="7" width="17.1796875" customWidth="1"/>
-    <col min="8" max="8" width="18.1796875" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" customWidth="1"/>
-    <col min="10" max="10" width="15.26953125" customWidth="1"/>
-    <col min="11" max="11" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" customWidth="1"/>
+    <col min="10" max="10" width="15.21875" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1067,13 +1092,13 @@
         <v>13</v>
       </c>
       <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1084,7 +1109,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
@@ -1099,16 +1124,16 @@
         <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1119,7 +1144,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>23</v>
@@ -1131,13 +1156,13 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1148,7 +1173,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>23</v>
@@ -1163,10 +1188,10 @@
         <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1177,7 +1202,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>23</v>
@@ -1189,19 +1214,19 @@
         <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1212,7 +1237,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>23</v>
@@ -1224,13 +1249,13 @@
         <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1241,7 +1266,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>23</v>
@@ -1253,7 +1278,7 @@
         <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
         <v>26</v>
@@ -1272,20 +1297,20 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" customWidth="1"/>
-    <col min="9" max="9" width="11.7265625" customWidth="1"/>
-    <col min="10" max="10" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1311,13 +1336,13 @@
         <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1328,7 +1353,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
@@ -1340,13 +1365,13 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1358,22 +1383,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
-    <col min="7" max="7" width="44.54296875" customWidth="1"/>
-    <col min="8" max="8" width="32.453125" customWidth="1"/>
+    <col min="7" max="7" width="44.5546875" customWidth="1"/>
+    <col min="8" max="8" width="32.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1399,7 +1424,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
@@ -1410,19 +1435,19 @@
         <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="F2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>